<commit_message>
updated citations to endnote
</commit_message>
<xml_diff>
--- a/NSSC lit log (1).xlsx
+++ b/NSSC lit log (1).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="390" windowWidth="21720" windowHeight="11430" activeTab="1"/>
+    <workbookView xWindow="330" yWindow="390" windowWidth="21720" windowHeight="11430"/>
   </bookViews>
   <sheets>
     <sheet name="Articles actually used" sheetId="1" r:id="rId1"/>
@@ -1156,9 +1156,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -1336,458 +1336,449 @@
     </row>
     <row r="9" spans="1:9" ht="37.5" customHeight="1">
       <c r="A9" s="4">
-        <v>2010</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>53</v>
+        <v>2013</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>241</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I9" s="7"/>
+        <v>242</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" ht="37.5" customHeight="1">
       <c r="A10" s="4">
         <v>2010</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
+      <c r="C10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="13"/>
     </row>
     <row r="11" spans="1:9" ht="37.5" customHeight="1">
       <c r="A11" s="4">
-        <v>2013</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I11" s="7"/>
+        <v>2010</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
     </row>
     <row r="12" spans="1:9" ht="37.5" customHeight="1">
       <c r="A12" s="4">
-        <v>2016</v>
+        <v>2013</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>40</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="40.5" customHeight="1">
       <c r="A13" s="4">
-        <v>2004</v>
+        <v>2016</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="37.5" customHeight="1">
       <c r="A14" s="4">
-        <v>2009</v>
+        <v>2004</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>58</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="37.5" customHeight="1">
       <c r="A15" s="4">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="F15" s="7"/>
-      <c r="G15" s="4" t="s">
-        <v>83</v>
-      </c>
+      <c r="G15" s="13"/>
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" ht="37.5" customHeight="1">
       <c r="A16" s="4">
-        <v>2010</v>
+        <v>2006</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9" ht="37.5" customHeight="1">
       <c r="A17" s="4">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G17" s="7"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9" ht="37.5" customHeight="1">
       <c r="A18" s="4">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+        <v>88</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="G18" s="7"/>
       <c r="I18" s="7"/>
     </row>
     <row r="19" spans="1:9" ht="37.5" customHeight="1">
       <c r="A19" s="4">
+        <v>2008</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="1:9" ht="37.5" customHeight="1">
+      <c r="A20" s="4">
         <v>2014</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B20" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C20" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D20" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E20" s="11" t="s">
         <v>94</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="37.5" customHeight="1">
-      <c r="A20" s="7">
-        <v>2013</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>103</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>95</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="H20" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="H20" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="37.5" customHeight="1">
       <c r="A21" s="7">
+        <v>2013</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="37.5" customHeight="1">
+      <c r="A22" s="13">
         <v>2010</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B22" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C22" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E22" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F22" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G22" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H22" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I21" s="4" t="s">
+      <c r="I22" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="37.5" customHeight="1">
-      <c r="A22" s="4">
-        <v>2002</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="I22" s="7"/>
     </row>
     <row r="23" spans="1:9" ht="37.5" customHeight="1">
       <c r="A23" s="4">
-        <v>2007</v>
+        <v>2001</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="I23" s="7"/>
+        <v>240</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9" ht="37.5" customHeight="1">
       <c r="A24" s="4">
-        <v>2005</v>
+        <v>2002</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>104</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="I24" s="7"/>
     </row>
     <row r="25" spans="1:9" ht="37.5" customHeight="1">
       <c r="A25" s="4">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>48</v>
+        <v>119</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>129</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="I25" s="13"/>
     </row>
     <row r="26" spans="1:9" ht="37.5" customHeight="1">
       <c r="A26" s="4">
-        <v>2016</v>
+        <v>2005</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>61</v>
+        <v>123</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>119</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="I26" s="7"/>
     </row>
     <row r="27" spans="1:9" ht="37.5" customHeight="1">
       <c r="A27" s="4">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="D27" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F27" s="7"/>
+      <c r="F27" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="G27" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="I27" s="7"/>
+        <v>129</v>
+      </c>
+      <c r="I27" s="4"/>
     </row>
     <row r="28" spans="1:9" ht="37.5" customHeight="1">
       <c r="A28" s="4">
-        <v>2008</v>
+        <v>2016</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>29</v>
+        <v>132</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F28" s="7"/>
+        <v>133</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="G28" s="4" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="I28" s="7"/>
     </row>
@@ -1796,34 +1787,42 @@
         <v>2004</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
+        <v>136</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="F29" s="7"/>
       <c r="G29" s="4" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="I29" s="7"/>
     </row>
     <row r="30" spans="1:9" ht="37.5" customHeight="1">
       <c r="A30" s="4">
-        <v>2003</v>
+        <v>2008</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
+        <v>139</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="F30" s="7"/>
       <c r="G30" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I30" s="7"/>
     </row>
@@ -1832,159 +1831,166 @@
         <v>2004</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>146</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" t="s">
+        <v>143</v>
+      </c>
+      <c r="I31" s="13"/>
     </row>
     <row r="32" spans="1:9" ht="37.5" customHeight="1">
       <c r="A32" s="4">
-        <v>2010</v>
+        <v>2003</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>62</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
       <c r="F32" s="7"/>
       <c r="G32" s="4" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="I32" s="7"/>
     </row>
     <row r="33" spans="1:9" ht="37.5" customHeight="1">
-      <c r="A33" s="7">
-        <v>2009</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="I33" s="7"/>
+      <c r="A33" s="4">
+        <v>2004</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="I33" s="4"/>
     </row>
     <row r="34" spans="1:9" ht="37.5" customHeight="1">
       <c r="A34" s="4">
-        <v>2013</v>
+        <v>2010</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>157</v>
+        <v>29</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>89</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="F34" s="13"/>
       <c r="G34" s="4" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="I34" s="7"/>
     </row>
     <row r="35" spans="1:9" ht="37.5" customHeight="1">
       <c r="A35" s="7">
-        <v>2013</v>
+        <v>2009</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="F35" s="10" t="s">
-        <v>95</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F35" s="10"/>
       <c r="G35" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="H35" s="4"/>
+      <c r="I35" s="13"/>
     </row>
     <row r="36" spans="1:9" ht="37.5" customHeight="1">
       <c r="A36" s="4">
-        <v>2010</v>
+        <v>2013</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>170</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="D36" t="s">
+        <v>157</v>
+      </c>
+      <c r="E36" t="s">
+        <v>158</v>
+      </c>
+      <c r="F36" t="s">
+        <v>89</v>
+      </c>
+      <c r="G36" t="s">
+        <v>159</v>
+      </c>
+      <c r="I36" s="13"/>
     </row>
     <row r="37" spans="1:9" ht="37.5" customHeight="1">
-      <c r="A37" s="4">
-        <v>2003</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="I37" s="7"/>
+      <c r="A37" s="13">
+        <v>2013</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="38" spans="1:9" ht="37.5" customHeight="1">
       <c r="A38" s="4">
-        <v>1998</v>
+        <v>2010</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="I38" s="7"/>
+        <v>170</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="I38" s="4"/>
     </row>
     <row r="39" spans="1:9" ht="37.5" customHeight="1">
       <c r="A39" s="4">
@@ -1994,255 +2000,283 @@
         <v>171</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
+        <v>172</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>173</v>
+      </c>
       <c r="I39" s="7"/>
     </row>
     <row r="40" spans="1:9" ht="37.5" customHeight="1">
       <c r="A40" s="4">
-        <v>2001</v>
+        <v>1998</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>179</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
       <c r="I40" s="7"/>
     </row>
     <row r="41" spans="1:9" ht="37.5" customHeight="1">
       <c r="A41" s="4">
-        <v>2007</v>
+        <v>2003</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>181</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="I41" s="13"/>
     </row>
     <row r="42" spans="1:9" ht="37.5" customHeight="1">
       <c r="A42" s="4">
-        <v>2016</v>
+        <v>2001</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>62</v>
+        <v>119</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>40</v>
+        <v>178</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="I42" s="7"/>
     </row>
     <row r="43" spans="1:9" ht="37.5" customHeight="1">
       <c r="A43" s="4">
-        <v>1999</v>
+        <v>2007</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="I43" s="7"/>
+        <v>181</v>
+      </c>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="I43" s="4"/>
     </row>
     <row r="44" spans="1:9" ht="37.5" customHeight="1">
       <c r="A44" s="4">
-        <v>2017</v>
+        <v>2008</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>191</v>
+        <v>237</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E44" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="1:9" ht="37.5" customHeight="1">
+      <c r="A45" s="4">
+        <v>2016</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E45" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F45" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G44" s="7"/>
-      <c r="I44" s="7"/>
-    </row>
-    <row r="45" spans="1:9" ht="37.5" customHeight="1">
-      <c r="A45" s="7">
-        <v>2015</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="F45" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="G45" s="12" t="s">
-        <v>197</v>
+      <c r="G45" s="4" t="s">
+        <v>184</v>
       </c>
       <c r="I45" s="7"/>
     </row>
     <row r="46" spans="1:9" ht="37.5" customHeight="1">
       <c r="A46" s="4">
-        <v>2004</v>
+        <v>1999</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
+        <v>186</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>189</v>
+      </c>
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
       <c r="I46" s="7"/>
     </row>
     <row r="47" spans="1:9" ht="37.5" customHeight="1">
       <c r="A47" s="4">
-        <v>2005</v>
+        <v>2017</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>202</v>
+        <v>61</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="F47" s="7"/>
+        <v>62</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="G47" s="7"/>
       <c r="I47" s="7"/>
     </row>
     <row r="48" spans="1:9" ht="37.5" customHeight="1">
-      <c r="A48" s="4">
+      <c r="A48" s="13">
+        <v>2015</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="I48" s="7"/>
+    </row>
+    <row r="49" spans="1:9" ht="37.5" customHeight="1">
+      <c r="A49" s="4">
+        <v>2004</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="I49" s="13"/>
+    </row>
+    <row r="50" spans="1:9" ht="37.5" customHeight="1">
+      <c r="A50" s="4">
+        <v>2005</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="D50" t="s">
+        <v>202</v>
+      </c>
+      <c r="E50" t="s">
+        <v>203</v>
+      </c>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="I50" s="13"/>
+    </row>
+    <row r="51" spans="1:9" ht="37.5" customHeight="1">
+      <c r="A51" s="4">
         <v>2008</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B51" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C51" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D51" t="s">
         <v>206</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E51" t="s">
         <v>48</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="F51" t="s">
         <v>196</v>
       </c>
-      <c r="G48" s="4" t="s">
+      <c r="G51" t="s">
         <v>207</v>
       </c>
-      <c r="I48" s="7"/>
-    </row>
-    <row r="49" spans="1:3" ht="37.5" customHeight="1">
-      <c r="A49" s="4">
+      <c r="I51" s="13"/>
+    </row>
+    <row r="52" spans="1:9" ht="37.5" customHeight="1">
+      <c r="A52" s="4">
         <v>2007</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B52" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C52" s="4" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="37.5" customHeight="1">
-      <c r="A50" s="4">
-        <v>2008</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="37.5" customHeight="1">
-      <c r="A51" s="4">
-        <v>2001</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="37.5" customHeight="1">
-      <c r="A52" s="4">
-        <v>2013</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="37.5" customHeight="1"/>
-    <row r="54" spans="1:3" ht="37.5" customHeight="1"/>
-    <row r="55" spans="1:3" ht="37.5" customHeight="1"/>
-    <row r="56" spans="1:3" ht="37.5" customHeight="1"/>
-    <row r="57" spans="1:3" ht="37.5" customHeight="1"/>
-    <row r="58" spans="1:3" ht="37.5" customHeight="1"/>
-    <row r="59" spans="1:3" ht="37.5" customHeight="1"/>
-    <row r="60" spans="1:3" ht="37.5" customHeight="1"/>
-    <row r="61" spans="1:3" ht="37.5" customHeight="1"/>
-    <row r="62" spans="1:3" ht="37.5" customHeight="1"/>
-    <row r="63" spans="1:3" ht="37.5" customHeight="1"/>
-    <row r="64" spans="1:3" ht="37.5" customHeight="1"/>
+    <row r="53" spans="1:9" ht="37.5" customHeight="1"/>
+    <row r="54" spans="1:9" ht="37.5" customHeight="1"/>
+    <row r="55" spans="1:9" ht="37.5" customHeight="1"/>
+    <row r="56" spans="1:9" ht="37.5" customHeight="1"/>
+    <row r="57" spans="1:9" ht="37.5" customHeight="1"/>
+    <row r="58" spans="1:9" ht="37.5" customHeight="1"/>
+    <row r="59" spans="1:9" ht="37.5" customHeight="1"/>
+    <row r="60" spans="1:9" ht="37.5" customHeight="1"/>
+    <row r="61" spans="1:9" ht="37.5" customHeight="1"/>
+    <row r="62" spans="1:9" ht="37.5" customHeight="1"/>
+    <row r="63" spans="1:9" ht="37.5" customHeight="1"/>
+    <row r="64" spans="1:9" ht="37.5" customHeight="1"/>
     <row r="65" ht="37.5" customHeight="1"/>
     <row r="66" ht="37.5" customHeight="1"/>
     <row r="67" ht="37.5" customHeight="1"/>
@@ -3179,6 +3213,9 @@
     <row r="998" ht="37.5" customHeight="1"/>
     <row r="999" ht="37.5" customHeight="1"/>
   </sheetData>
+  <sortState ref="A2:I999">
+    <sortCondition ref="B2:B999"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3187,9 +3224,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -13342,6 +13379,9 @@
       <c r="K999" s="7"/>
     </row>
   </sheetData>
+  <sortState ref="A2:K999">
+    <sortCondition ref="D2:D999"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>